<commit_message>
synching create tables with create all
</commit_message>
<xml_diff>
--- a/Database/Documentation/CRUD_matrix.xlsx
+++ b/Database/Documentation/CRUD_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitHubRepos_4\Siba23k\Siba_be\Database\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3033138-D434-4B4A-9AC9-5873D29D6116}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9145F09-7E8D-4C2A-97C6-8910B4EEF377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7490" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19164" windowHeight="7488" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,9 +81,6 @@
     <t>Delete</t>
   </si>
   <si>
-    <t>Execute database procedure</t>
-  </si>
-  <si>
     <t>Alloc* (other tables)</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>?CRUD</t>
+  </si>
+  <si>
+    <t>Execute database procedure/trigger</t>
   </si>
 </sst>
 </file>
@@ -543,17 +543,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EDD8D4-768F-4459-BFF7-F89017F48637}">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="15.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="15.77734375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,7 +567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -590,9 +590,9 @@
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -615,12 +615,12 @@
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
@@ -634,7 +634,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="12"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -649,7 +649,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
@@ -672,9 +672,9 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
@@ -688,14 +688,14 @@
         <v>10</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -706,9 +706,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
@@ -719,16 +719,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -739,39 +739,39 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
-        <v>25</v>
-      </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>5</v>
@@ -780,9 +780,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -797,9 +797,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
@@ -814,16 +814,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="11"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>4</v>
@@ -834,9 +834,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>
@@ -847,19 +847,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="11"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -867,12 +867,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -880,12 +880,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -893,16 +893,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="11"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>4</v>
@@ -913,72 +913,72 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="11"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="11"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fine-tuning the CRUD matrix excel
</commit_message>
<xml_diff>
--- a/Database/Documentation/CRUD_matrix.xlsx
+++ b/Database/Documentation/CRUD_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitHubRepos_4\Siba23k\Siba_be\Database\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9145F09-7E8D-4C2A-97C6-8910B4EEF377}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FF798F-35BC-434B-906E-A25F17E145B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19164" windowHeight="7488" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7490" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
   <si>
     <t>Admin</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Plan.(in general)</t>
   </si>
   <si>
-    <t>Only stored proc</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>DepartmentPlanner</t>
   </si>
   <si>
-    <t>AllocRoundUser</t>
-  </si>
-  <si>
     <t>log_event</t>
   </si>
   <si>
@@ -139,6 +133,18 @@
   </si>
   <si>
     <t>Execute database procedure/trigger</t>
+  </si>
+  <si>
+    <t>X (Only stored proc)</t>
+  </si>
+  <si>
+    <t>AllocRoundCurrentUser</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Confirm from Customer</t>
   </si>
 </sst>
 </file>
@@ -544,16 +550,16 @@
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="15.77734375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="16.6328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -567,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
@@ -582,24 +588,22 @@
         <v>5</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
@@ -610,21 +614,21 @@
         <v>5</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="9"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>5</v>
@@ -634,22 +638,22 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="G5" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
@@ -664,125 +668,139 @@
         <v>5</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="G9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="11"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="11"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A14" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -797,9 +815,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
@@ -814,16 +832,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="11"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>4</v>
@@ -834,151 +852,161 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E19" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="11"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="11" t="s">
+      <c r="B23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="D23" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E23" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="11"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="D25" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E25" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="11"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="11"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New version of CRUDL matrix. Some todo markers
</commit_message>
<xml_diff>
--- a/Database/Documentation/CRUD_matrix.xlsx
+++ b/Database/Documentation/CRUD_matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitHubRepos_4\Siba23k\Siba_be\Database\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitRepos\Siba\Siba_be\Database\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FF798F-35BC-434B-906E-A25F17E145B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5D42A3-5EF9-4D71-B607-749E12FB6DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19160" windowHeight="7490" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="44">
   <si>
     <t>Admin</t>
   </si>
@@ -132,9 +132,6 @@
     <t>?CRUD</t>
   </si>
   <si>
-    <t>Execute database procedure/trigger</t>
-  </si>
-  <si>
     <t>X (Only stored proc)</t>
   </si>
   <si>
@@ -144,7 +141,22 @@
     <t>?</t>
   </si>
   <si>
-    <t>Confirm from Customer</t>
+    <t>Execute procedure/trigger</t>
+  </si>
+  <si>
+    <t>DCA</t>
+  </si>
+  <si>
+    <t>(child only)</t>
+  </si>
+  <si>
+    <t>DNA</t>
+  </si>
+  <si>
+    <t>FK policy Del (if this Mother row tried to delete)</t>
+  </si>
+  <si>
+    <t>Confirmation asked from Customer</t>
   </si>
 </sst>
 </file>
@@ -203,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,23 +227,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,19 +553,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EDD8D4-768F-4459-BFF7-F89017F48637}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="16.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.81640625" customWidth="1"/>
+    <col min="7" max="7" width="4.26953125" customWidth="1"/>
+    <col min="8" max="8" width="30.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -572,9 +582,12 @@
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
+      <c r="I1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -587,21 +600,22 @@
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="11" t="s">
+      <c r="I2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
@@ -610,18 +624,19 @@
       <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="11" t="s">
-        <v>37</v>
+      <c r="I3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>31</v>
@@ -633,28 +648,26 @@
       <c r="E4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="12"/>
+      <c r="G4" s="1"/>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="7"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -667,17 +680,18 @@
       <c r="E6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="11" t="s">
+      <c r="I6" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -690,17 +704,18 @@
       <c r="E7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="11" t="s">
+      <c r="H7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -713,9 +728,12 @@
       <c r="E8" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="11" t="s">
+      <c r="I8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -728,22 +746,25 @@
       <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A10" s="11"/>
+      <c r="G9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -756,16 +777,19 @@
       <c r="E11" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" s="11"/>
+      <c r="I11" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="6"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -780,9 +804,12 @@
       <c r="E13" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="11" t="s">
+      <c r="I13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
         <v>23</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -797,15 +824,18 @@
       <c r="E14" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" s="11" t="s">
+      <c r="I14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -814,15 +844,18 @@
       <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="I15" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -831,29 +864,37 @@
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="11"/>
+      <c r="I16" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="D18" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="E18" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="I18" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -866,16 +907,19 @@
       <c r="E19" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
+      <c r="I19" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="6"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>28</v>
       </c>
       <c r="B21" s="4" t="s">
@@ -889,8 +933,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B22" s="4" t="s">
@@ -904,8 +948,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -919,15 +963,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="11"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="6"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="4" t="s">
@@ -941,33 +985,33 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="11"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="6"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="11"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="6"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
CRUD_matrix updated based on customer's responses. No big changes.
</commit_message>
<xml_diff>
--- a/Database/Documentation/CRUD_matrix.xlsx
+++ b/Database/Documentation/CRUD_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitRepos\Siba\Siba_be\Database\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5D42A3-5EF9-4D71-B607-749E12FB6DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0472D488-C4FF-4B90-9CAB-B98187C8C58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
   <si>
     <t>Admin</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Planner(ownDep)</t>
   </si>
   <si>
-    <t>?R</t>
-  </si>
-  <si>
     <t>Plan.(in general)</t>
   </si>
   <si>
@@ -129,18 +126,12 @@
     <t>GlobalStting</t>
   </si>
   <si>
-    <t>?CRUD</t>
-  </si>
-  <si>
     <t>X (Only stored proc)</t>
   </si>
   <si>
     <t>AllocRoundCurrentUser</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Execute procedure/trigger</t>
   </si>
   <si>
@@ -156,7 +147,7 @@
     <t>FK policy Del (if this Mother row tried to delete)</t>
   </si>
   <si>
-    <t>Confirmation asked from Customer</t>
+    <t>Confirm from Customer 2024-02-06</t>
   </si>
 </sst>
 </file>
@@ -180,12 +171,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -215,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -237,6 +234,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -555,7 +561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EDD8D4-768F-4459-BFF7-F89017F48637}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -577,13 +583,13 @@
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -601,21 +607,21 @@
         <v>5</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
@@ -628,18 +634,18 @@
         <v>5</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
@@ -650,7 +656,7 @@
       </c>
       <c r="G4" s="1"/>
       <c r="I4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
@@ -660,10 +666,10 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
@@ -681,18 +687,18 @@
         <v>5</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>4</v>
@@ -705,18 +711,18 @@
         <v>5</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H7" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -729,12 +735,12 @@
         <v>5</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
@@ -746,14 +752,12 @@
       <c r="E9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="G9" s="11"/>
       <c r="H9" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
@@ -765,7 +769,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -778,7 +782,7 @@
         <v>5</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
@@ -790,7 +794,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>4</v>
@@ -798,39 +802,39 @@
       <c r="C13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>7</v>
+      <c r="D13" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>7</v>
+      <c r="C14" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -838,19 +842,19 @@
       <c r="C15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>7</v>
+      <c r="D15" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>4</v>
@@ -858,14 +862,14 @@
       <c r="C16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>7</v>
+      <c r="D16" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -877,25 +881,25 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="4" t="s">
-        <v>37</v>
+      <c r="D18" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>4</v>
@@ -908,7 +912,7 @@
         <v>5</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -920,10 +924,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4" t="s">
@@ -935,10 +939,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
@@ -950,10 +954,10 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4" t="s">
@@ -972,7 +976,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
upd CRUDL matrix again
</commit_message>
<xml_diff>
--- a/Database/Documentation/CRUD_matrix.xlsx
+++ b/Database/Documentation/CRUD_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitRepos\Siba\Siba_be\Database\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0472D488-C4FF-4B90-9CAB-B98187C8C58F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C6B243-42D2-4E70-8710-FBCC0457C86D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="42">
   <si>
     <t>Admin</t>
   </si>
@@ -147,7 +147,10 @@
     <t>FK policy Del (if this Mother row tried to delete)</t>
   </si>
   <si>
-    <t>Confirm from Customer 2024-02-06</t>
+    <t>Confirmed from the …</t>
+  </si>
+  <si>
+    <t>… Customer 2024-02-06</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +184,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -212,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -245,6 +254,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,7 +575,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -766,6 +779,10 @@
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
@@ -775,8 +792,8 @@
         <v>4</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
+      <c r="D11" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Another update to CRUD matrix from customer, planners cannot change spaces nor their equipment
</commit_message>
<xml_diff>
--- a/Database/Documentation/CRUD_matrix.xlsx
+++ b/Database/Documentation/CRUD_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitRepos\Siba\Siba_be\Database\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEACDBF-F33B-4E68-B808-E9E4384F236E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C06D34-CC6F-410D-ABF3-3CEEFC9F18C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
   <si>
     <t>Admin</t>
   </si>
@@ -151,12 +151,6 @@
   </si>
   <si>
     <t>… Customer 2024-02-06</t>
-  </si>
-  <si>
-    <t>CRUD?</t>
-  </si>
-  <si>
-    <t>R / CRUD?</t>
   </si>
   <si>
     <t>What about these?</t>
@@ -594,7 +588,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,7 +731,7 @@
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="14" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>5</v>
@@ -761,7 +755,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="14" t="s">
-        <v>42</v>
+        <v>5</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>5</v>
@@ -829,7 +823,7 @@
       <c r="E12" s="4"/>
       <c r="G12" s="15"/>
       <c r="H12" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
linter rule for noUselessElse turned off. CRUD excel small update
</commit_message>
<xml_diff>
--- a/Database/Documentation/CRUD_matrix.xlsx
+++ b/Database/Documentation/CRUD_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_GitRepos\Siba\Siba_be\Database\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C06D34-CC6F-410D-ABF3-3CEEFC9F18C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55355758-0CDD-4B2F-82A0-C2B4F35E1C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{F42ABF6E-CD7D-4AD6-B90F-5AA9FC69C429}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="44">
   <si>
     <t>Admin</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>What about these?</t>
+  </si>
+  <si>
+    <t>U: Planner cannot change name</t>
   </si>
 </sst>
 </file>
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EDD8D4-768F-4459-BFF7-F89017F48637}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -601,7 +604,7 @@
     <col min="9" max="9" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -618,7 +621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -642,7 +645,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>16</v>
       </c>
@@ -666,7 +669,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -685,7 +688,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -698,7 +701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -722,7 +725,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>17</v>
       </c>
@@ -746,7 +749,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -764,7 +767,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>19</v>
       </c>
@@ -786,7 +789,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="6"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -797,7 +800,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>20</v>
       </c>
@@ -814,8 +817,11 @@
       <c r="I11" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -826,7 +832,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
@@ -846,7 +852,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>22</v>
       </c>
@@ -866,7 +872,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>24</v>
       </c>
@@ -886,7 +892,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>23</v>
       </c>

</xml_diff>